<commit_message>
增加了对寄存器组的规定 / Added provisions for register groups
</commit_message>
<xml_diff>
--- a/image/指令集.xlsx
+++ b/image/指令集.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="53">
   <si>
     <t>短指令</t>
   </si>
@@ -46,7 +46,7 @@
     <t>长指令</t>
   </si>
   <si>
-    <t>rom/ram_addr/immediate</t>
+    <t>rom_addr/ram_addr/immediate</t>
   </si>
   <si>
     <t>NOP</t>
@@ -67,7 +67,7 @@
     <t>关机(其中XXXX不能全为0)</t>
   </si>
   <si>
-    <t>B</t>
+    <t>B    immediate</t>
   </si>
   <si>
     <t>8'b0001_XXXX</t>
@@ -79,7 +79,7 @@
     <t>无条件转移</t>
   </si>
   <si>
-    <t>BEQ</t>
+    <t>BEQ  immediate</t>
   </si>
   <si>
     <t>8'b0010_XXXX</t>
@@ -88,7 +88,7 @@
     <t>等于转移(ac_out==reg_out时)</t>
   </si>
   <si>
-    <t>BLT</t>
+    <t>BLT  immediate</t>
   </si>
   <si>
     <t>8'b0011_XXXX</t>
@@ -97,7 +97,7 @@
     <t>小于转移(ac_out&lt;reg_out时)</t>
   </si>
   <si>
-    <t>LDO</t>
+    <t>LDO  rom_addr</t>
   </si>
   <si>
     <t>8'b0101_XXXX</t>
@@ -106,7 +106,7 @@
     <t>AC &lt;- ROM[addr]</t>
   </si>
   <si>
-    <t>LDA</t>
+    <t>LDA  ram_addr</t>
   </si>
   <si>
     <t>8'b0110_XXXX</t>
@@ -115,7 +115,7 @@
     <t>AC &lt;- RAM[addr]</t>
   </si>
   <si>
-    <t>STO</t>
+    <t>STO  reg_addr, ram_addr</t>
   </si>
   <si>
     <t>8'b0111_XXXX</t>
@@ -124,7 +124,7 @@
     <t>RAM &lt;- REG[reg_addr]</t>
   </si>
   <si>
-    <t>PRE</t>
+    <t>PRE  reg_addr</t>
   </si>
   <si>
     <t>8'b1001_XXXX</t>
@@ -133,7 +133,7 @@
     <t>REG[reg_addr] &lt;- AC</t>
   </si>
   <si>
-    <t>LDM</t>
+    <t>LDM  reg_addr</t>
   </si>
   <si>
     <t>8'b1010_XXXX</t>
@@ -142,7 +142,7 @@
     <t>AC &lt;- REG[reg_addr]</t>
   </si>
   <si>
-    <t>ADDI</t>
+    <t>ADDI immediate</t>
   </si>
   <si>
     <t>8'b1100_XXXX</t>
@@ -157,7 +157,7 @@
     <t>AC =~AC</t>
   </si>
   <si>
-    <t>ADD</t>
+    <t>ADD  reg_addr</t>
   </si>
   <si>
     <t>8'b1101_XXXX</t>
@@ -166,7 +166,7 @@
     <t>AC = AC + reg_out</t>
   </si>
   <si>
-    <t>LS</t>
+    <t>LS   reg_addr</t>
   </si>
   <si>
     <t>8'b1110_XXXX</t>
@@ -175,13 +175,19 @@
     <t>AC = AC &lt;&lt; reg_out</t>
   </si>
   <si>
-    <t>RS</t>
+    <t>RS   reg_addr</t>
   </si>
   <si>
     <t>8'b1111_XXXX</t>
   </si>
   <si>
     <t>AC = AC &gt;&gt; reg_out</t>
+  </si>
+  <si>
+    <t>SUB  reg_addr</t>
+  </si>
+  <si>
+    <t>AC = AC - reg_out</t>
   </si>
 </sst>
 </file>
@@ -194,7 +200,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -204,6 +210,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="6"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -757,139 +770,142 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -921,6 +937,15 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -929,6 +954,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
@@ -1247,527 +1275,598 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:Q20"/>
+  <dimension ref="A1:Q31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
+    <col min="1" max="1" width="21.925" customWidth="1"/>
     <col min="2" max="17" width="3.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" spans="1:9">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1" t="s">
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
     </row>
     <row r="2" ht="14.25" spans="2:9">
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2" s="11" t="s">
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="15" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" ht="14.25" spans="1:17">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1" t="s">
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1" t="s">
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-    </row>
-    <row r="4" ht="14.25" spans="2:17">
-      <c r="B4" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J4" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="K4" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="L4" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="M4" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="N4" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="O4" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="P4" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q4" s="14" t="s">
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+    </row>
+    <row r="4" spans="2:17">
+      <c r="B4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="L4" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="M4" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="N4" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="O4" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="P4" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q4" s="19" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:17">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="13" t="s">
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="13"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="13"/>
-      <c r="P6" s="13"/>
-      <c r="Q6" s="15"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="17"/>
+      <c r="O6" s="17"/>
+      <c r="P6" s="17"/>
+      <c r="Q6" s="20"/>
     </row>
     <row r="7" spans="1:17">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="13" t="s">
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="13"/>
-      <c r="P7" s="13"/>
-      <c r="Q7" s="13"/>
+      <c r="K7" s="17"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="17"/>
+      <c r="N7" s="17"/>
+      <c r="O7" s="17"/>
+      <c r="P7" s="17"/>
+      <c r="Q7" s="17"/>
     </row>
     <row r="8" spans="1:17">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="10" t="s">
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="13" t="s">
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="13"/>
-      <c r="O8" s="13"/>
-      <c r="P8" s="13"/>
-      <c r="Q8" s="13"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="17"/>
+      <c r="N8" s="17"/>
+      <c r="O8" s="17"/>
+      <c r="P8" s="17"/>
+      <c r="Q8" s="17"/>
     </row>
     <row r="9" spans="1:17">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="10" t="s">
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="13" t="s">
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="13"/>
-      <c r="O9" s="13"/>
-      <c r="P9" s="13"/>
-      <c r="Q9" s="13"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="17"/>
+      <c r="P9" s="17"/>
+      <c r="Q9" s="17"/>
     </row>
     <row r="10" spans="1:17">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="10" t="s">
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="13" t="s">
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
-      <c r="N10" s="13"/>
-      <c r="O10" s="13"/>
-      <c r="P10" s="13"/>
-      <c r="Q10" s="13"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="17"/>
+      <c r="N10" s="17"/>
+      <c r="O10" s="17"/>
+      <c r="P10" s="17"/>
+      <c r="Q10" s="17"/>
     </row>
     <row r="11" spans="1:17">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="10" t="s">
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="13" t="s">
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="13"/>
-      <c r="N11" s="13"/>
-      <c r="O11" s="13"/>
-      <c r="P11" s="13"/>
-      <c r="Q11" s="13"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="17"/>
+      <c r="N11" s="17"/>
+      <c r="O11" s="17"/>
+      <c r="P11" s="17"/>
+      <c r="Q11" s="17"/>
     </row>
     <row r="12" spans="1:17">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="10" t="s">
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="13" t="s">
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="13"/>
-      <c r="N12" s="13"/>
-      <c r="O12" s="13"/>
-      <c r="P12" s="13"/>
-      <c r="Q12" s="13"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="17"/>
+      <c r="O12" s="17"/>
+      <c r="P12" s="17"/>
+      <c r="Q12" s="17"/>
     </row>
     <row r="13" spans="1:17">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="10" t="s">
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="13" t="s">
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
-      <c r="N13" s="13"/>
-      <c r="O13" s="13"/>
-      <c r="P13" s="13"/>
-      <c r="Q13" s="13"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="17"/>
+      <c r="N13" s="17"/>
+      <c r="O13" s="17"/>
+      <c r="P13" s="17"/>
+      <c r="Q13" s="17"/>
     </row>
     <row r="14" spans="1:17">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="13" t="s">
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="13"/>
-      <c r="N14" s="13"/>
-      <c r="O14" s="13"/>
-      <c r="P14" s="13"/>
-      <c r="Q14" s="13"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="17"/>
+      <c r="M14" s="17"/>
+      <c r="N14" s="17"/>
+      <c r="O14" s="17"/>
+      <c r="P14" s="17"/>
+      <c r="Q14" s="17"/>
     </row>
     <row r="15" spans="1:17">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="13" t="s">
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="13"/>
-      <c r="N15" s="13"/>
-      <c r="O15" s="13"/>
-      <c r="P15" s="13"/>
-      <c r="Q15" s="13"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="17"/>
+      <c r="N15" s="17"/>
+      <c r="O15" s="17"/>
+      <c r="P15" s="17"/>
+      <c r="Q15" s="17"/>
     </row>
     <row r="16" spans="1:17">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="10" t="s">
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="13" t="s">
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="13"/>
-      <c r="N16" s="13"/>
-      <c r="O16" s="13"/>
-      <c r="P16" s="13"/>
-      <c r="Q16" s="13"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
+      <c r="N16" s="17"/>
+      <c r="O16" s="17"/>
+      <c r="P16" s="17"/>
+      <c r="Q16" s="17"/>
     </row>
     <row r="17" spans="1:17">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="10" t="s">
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="13" t="s">
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="13"/>
-      <c r="N17" s="13"/>
-      <c r="O17" s="13"/>
-      <c r="P17" s="13"/>
-      <c r="Q17" s="13"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="17"/>
+      <c r="N17" s="17"/>
+      <c r="O17" s="17"/>
+      <c r="P17" s="17"/>
+      <c r="Q17" s="17"/>
     </row>
     <row r="18" spans="1:17">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="13" t="s">
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="K18" s="13"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="13"/>
-      <c r="N18" s="13"/>
-      <c r="O18" s="13"/>
-      <c r="P18" s="13"/>
-      <c r="Q18" s="13"/>
+      <c r="K18" s="17"/>
+      <c r="L18" s="17"/>
+      <c r="M18" s="17"/>
+      <c r="N18" s="17"/>
+      <c r="O18" s="17"/>
+      <c r="P18" s="17"/>
+      <c r="Q18" s="17"/>
     </row>
     <row r="19" spans="1:17">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="13" t="s">
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="K19" s="13"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="13"/>
-      <c r="N19" s="13"/>
-      <c r="O19" s="13"/>
-      <c r="P19" s="13"/>
-      <c r="Q19" s="13"/>
+      <c r="K19" s="17"/>
+      <c r="L19" s="17"/>
+      <c r="M19" s="17"/>
+      <c r="N19" s="17"/>
+      <c r="O19" s="17"/>
+      <c r="P19" s="17"/>
+      <c r="Q19" s="17"/>
     </row>
     <row r="20" spans="1:17">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="13" t="s">
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="13"/>
-      <c r="N20" s="13"/>
-      <c r="O20" s="13"/>
-      <c r="P20" s="13"/>
-      <c r="Q20" s="13"/>
+      <c r="K20" s="17"/>
+      <c r="L20" s="17"/>
+      <c r="M20" s="17"/>
+      <c r="N20" s="17"/>
+      <c r="O20" s="17"/>
+      <c r="P20" s="17"/>
+      <c r="Q20" s="17"/>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="13"/>
+      <c r="F21" s="14"/>
+      <c r="J21" s="18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="12"/>
+      <c r="B22" s="13"/>
+      <c r="F22" s="14"/>
+      <c r="J22" s="18"/>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="12"/>
+      <c r="B23" s="13"/>
+      <c r="F23" s="14"/>
+      <c r="J23" s="18"/>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="12"/>
+      <c r="B24" s="13"/>
+      <c r="F24" s="14"/>
+      <c r="J24" s="18"/>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="12"/>
+      <c r="B25" s="13"/>
+      <c r="F25" s="14"/>
+      <c r="J25" s="18"/>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="12"/>
+      <c r="B26" s="13"/>
+      <c r="F26" s="14"/>
+      <c r="J26" s="18"/>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="12"/>
+      <c r="B27" s="13"/>
+      <c r="F27" s="14"/>
+      <c r="J27" s="18"/>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="12"/>
+      <c r="B28" s="13"/>
+      <c r="F28" s="14"/>
+      <c r="J28" s="18"/>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" s="12"/>
+      <c r="B29" s="13"/>
+      <c r="F29" s="14"/>
+      <c r="J29" s="18"/>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" s="12"/>
+      <c r="B30" s="13"/>
+      <c r="F30" s="14"/>
+      <c r="J30" s="18"/>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" s="12"/>
+      <c r="B31" s="13"/>
+      <c r="F31" s="14"/>
+      <c r="J31" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="27">

</xml_diff>